<commit_message>
Added dummy clinic details
</commit_message>
<xml_diff>
--- a/raw_data/user_and_data_parameters/user_and_data_params.xlsx
+++ b/raw_data/user_and_data_parameters/user_and_data_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew_Eves\Documents\HSMA_local\Greener NHS funded development\shine\raw_data\user_and_data_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uclpartners-my.sharepoint.com/personal/sarah_houston_uclpartners_com/Documents/Other/Desktop/GH Clones/SHINE/shine/raw_data/user_and_data_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD252D3C-02D0-4337-BB9F-F4A13B527A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BD252D3C-02D0-4337-BB9F-F4A13B527A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70F80642-F5B1-490C-BFC3-AC8A753852B0}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1575" windowWidth="38700" windowHeight="15105" tabRatio="722" firstSheet="2" activeTab="3" xr2:uid="{24475980-04B6-4043-8A41-34925FD08545}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="2" activeTab="7" xr2:uid="{24475980-04B6-4043-8A41-34925FD08545}"/>
   </bookViews>
   <sheets>
     <sheet name="AssignFieldNamesToVars" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="554">
   <si>
     <t>field_name_in_service_data</t>
   </si>
@@ -2635,6 +2635,36 @@
   </si>
   <si>
     <t>Test Service</t>
+  </si>
+  <si>
+    <t>FNCH</t>
+  </si>
+  <si>
+    <t>DE223NE</t>
+  </si>
+  <si>
+    <t>Peartree Clinic</t>
+  </si>
+  <si>
+    <t>DE236QD</t>
+  </si>
+  <si>
+    <t>Whitworth Hospital</t>
+  </si>
+  <si>
+    <t>DE42JD</t>
+  </si>
+  <si>
+    <t>Alfreton Primary Care Centre</t>
+  </si>
+  <si>
+    <t>DE557AH</t>
+  </si>
+  <si>
+    <t>Ashbourne Clinic</t>
+  </si>
+  <si>
+    <t>DE61DR</t>
   </si>
 </sst>
 </file>
@@ -2933,7 +2963,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3047,13 +3077,12 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4187,7 +4216,7 @@
       <c r="A2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B2" s="58"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="8" t="s">
         <v>314</v>
       </c>
@@ -4234,10 +4263,10 @@
       <c r="A3" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C3" s="59">
+      <c r="C3" s="58">
         <v>0</v>
       </c>
       <c r="F3" s="37"/>
@@ -4246,10 +4275,10 @@
       <c r="A4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="58">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="F4" s="37"/>
@@ -4258,10 +4287,10 @@
       <c r="A5" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>0.77800000000000002</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="58">
         <v>0.17199999999999999</v>
       </c>
       <c r="F5" s="37"/>
@@ -4270,10 +4299,10 @@
       <c r="A6" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="58">
         <v>0.183</v>
       </c>
       <c r="D6" s="23"/>
@@ -4283,10 +4312,10 @@
       <c r="A7" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="58">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="59">
+      <c r="C7" s="58">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="D7" s="37"/>
@@ -4296,10 +4325,10 @@
       <c r="A8" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="58">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="58">
         <v>0</v>
       </c>
       <c r="D8" s="37"/>
@@ -4410,25 +4439,25 @@
       <c r="A4" s="51" t="s">
         <v>323</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="58">
         <v>0</v>
       </c>
-      <c r="D4" s="59">
+      <c r="D4" s="58">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="58">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="58">
         <v>0</v>
       </c>
-      <c r="G4" s="59">
+      <c r="G4" s="58">
         <v>0</v>
       </c>
-      <c r="H4" s="59">
+      <c r="H4" s="58">
         <v>0</v>
       </c>
       <c r="J4" s="50" t="s">
@@ -4457,25 +4486,25 @@
       <c r="A5" s="51" t="s">
         <v>324</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="58">
         <v>5.5E-2</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="58">
         <v>0.13100000000000001</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="58">
         <v>0.13300000000000001</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="58">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="58">
         <v>4.7E-2</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="58">
         <v>0.17346</v>
       </c>
     </row>
@@ -4483,25 +4512,25 @@
       <c r="A6" s="52" t="s">
         <v>490</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <v>0.77799999999999991</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="58">
         <v>0.5</v>
       </c>
-      <c r="D6" s="59">
+      <c r="D6" s="58">
         <v>0.77700000000000002</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="58">
         <v>0.82399999999999995</v>
       </c>
-      <c r="F6" s="59">
+      <c r="F6" s="58">
         <v>0.93700000000000006</v>
       </c>
-      <c r="G6" s="59">
+      <c r="G6" s="58">
         <v>0.95299999999999996</v>
       </c>
-      <c r="H6" s="59">
+      <c r="H6" s="58">
         <v>0.27435999999999999</v>
       </c>
     </row>
@@ -4509,25 +4538,25 @@
       <c r="A7" s="51" t="s">
         <v>326</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="59">
+      <c r="C7" s="58">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="58">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="58">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="58">
         <v>0</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="58">
         <v>0.18274000000000001</v>
       </c>
     </row>
@@ -4535,25 +4564,25 @@
       <c r="A8" s="51" t="s">
         <v>327</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="58">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="58">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="58">
         <v>0</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="58">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="58">
         <v>0</v>
       </c>
-      <c r="H8" s="59">
+      <c r="H8" s="58">
         <v>5.7119999999999997E-2</v>
       </c>
     </row>
@@ -4561,25 +4590,25 @@
       <c r="A9" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="58">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="58">
         <v>0.42299999999999999</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="58">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="58">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="58">
         <v>0</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="58">
         <v>0</v>
       </c>
-      <c r="H9" s="59">
+      <c r="H9" s="58">
         <v>0</v>
       </c>
     </row>
@@ -6959,7 +6988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02862E97-ED6B-45A0-9477-766967619C86}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7167,7 +7196,7 @@
       <c r="H7" s="43" t="s">
         <v>341</v>
       </c>
-      <c r="I7" s="57">
+      <c r="I7" s="56">
         <v>0.5</v>
       </c>
       <c r="J7" s="43">
@@ -7195,7 +7224,7 @@
       <c r="H8" s="43" t="s">
         <v>343</v>
       </c>
-      <c r="I8" s="57">
+      <c r="I8" s="56">
         <v>0.5</v>
       </c>
       <c r="J8" s="43">
@@ -7213,7 +7242,7 @@
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
       <c r="H9" s="43"/>
-      <c r="I9" s="57"/>
+      <c r="I9" s="56"/>
       <c r="J9" s="43"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7227,7 +7256,7 @@
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
       <c r="H10" s="43"/>
-      <c r="I10" s="57"/>
+      <c r="I10" s="56"/>
       <c r="J10" s="43"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -7241,7 +7270,7 @@
       <c r="F11" s="47"/>
       <c r="G11" s="47"/>
       <c r="H11" s="43"/>
-      <c r="I11" s="57"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -7255,7 +7284,7 @@
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
       <c r="H12" s="43"/>
-      <c r="I12" s="57"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="43"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -7269,7 +7298,7 @@
       <c r="F13" s="47"/>
       <c r="G13" s="47"/>
       <c r="H13" s="43"/>
-      <c r="I13" s="57"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="43"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -7283,7 +7312,7 @@
       <c r="F14" s="47"/>
       <c r="G14" s="47"/>
       <c r="H14" s="43"/>
-      <c r="I14" s="57"/>
+      <c r="I14" s="56"/>
       <c r="J14" s="43"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -7297,7 +7326,7 @@
       <c r="F15" s="47"/>
       <c r="G15" s="47"/>
       <c r="H15" s="43"/>
-      <c r="I15" s="57"/>
+      <c r="I15" s="56"/>
       <c r="J15" s="43"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -7311,7 +7340,7 @@
       <c r="F16" s="47"/>
       <c r="G16" s="47"/>
       <c r="H16" s="43"/>
-      <c r="I16" s="57"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="43"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -7325,7 +7354,7 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="43"/>
-      <c r="I17" s="57"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="43"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -7339,7 +7368,7 @@
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
       <c r="H18" s="43"/>
-      <c r="I18" s="57"/>
+      <c r="I18" s="56"/>
       <c r="J18" s="43"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -7353,7 +7382,7 @@
       <c r="F19" s="47"/>
       <c r="G19" s="47"/>
       <c r="H19" s="43"/>
-      <c r="I19" s="57"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -7367,7 +7396,7 @@
       <c r="F20" s="47"/>
       <c r="G20" s="47"/>
       <c r="H20" s="43"/>
-      <c r="I20" s="57"/>
+      <c r="I20" s="56"/>
       <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -7381,7 +7410,7 @@
       <c r="F21" s="47"/>
       <c r="G21" s="47"/>
       <c r="H21" s="43"/>
-      <c r="I21" s="57"/>
+      <c r="I21" s="56"/>
       <c r="J21" s="43"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -7395,7 +7424,7 @@
       <c r="F22" s="47"/>
       <c r="G22" s="47"/>
       <c r="H22" s="43"/>
-      <c r="I22" s="57"/>
+      <c r="I22" s="56"/>
       <c r="J22" s="43"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -7409,7 +7438,7 @@
       <c r="F23" s="47"/>
       <c r="G23" s="47"/>
       <c r="H23" s="43"/>
-      <c r="I23" s="57"/>
+      <c r="I23" s="56"/>
       <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -7423,7 +7452,7 @@
       <c r="F24" s="47"/>
       <c r="G24" s="47"/>
       <c r="H24" s="43"/>
-      <c r="I24" s="57"/>
+      <c r="I24" s="56"/>
       <c r="J24" s="43"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7437,7 +7466,7 @@
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
       <c r="H25" s="43"/>
-      <c r="I25" s="57"/>
+      <c r="I25" s="56"/>
       <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -7451,7 +7480,7 @@
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
       <c r="H26" s="43"/>
-      <c r="I26" s="57"/>
+      <c r="I26" s="56"/>
       <c r="J26" s="43"/>
     </row>
   </sheetData>
@@ -8128,8 +8157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4543EF9-90B8-43D4-9F53-935431C415A2}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8167,29 +8196,59 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -8599,13 +8658,6 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-    </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
         <v>519</v>
@@ -8705,7 +8757,7 @@
       <c r="A57" s="54" t="s">
         <v>534</v>
       </c>
-      <c r="B57" s="56" t="s">
+      <c r="B57" s="55" t="s">
         <v>535</v>
       </c>
     </row>

</xml_diff>